<commit_message>
Rewriting portfolio optimization section
</commit_message>
<xml_diff>
--- a/Docs/TargetDirectory.xlsx
+++ b/Docs/TargetDirectory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\denni\OneDrive\DelesinDJI\DDJI\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="6_{75A2AFA7-0ECF-4D0B-9C44-CA080D06DF9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B3E72FCA-3ADE-4054-B91A-0605DC1AA129}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="6_{75A2AFA7-0ECF-4D0B-9C44-CA080D06DF9B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{5D2F9AFC-2A62-46C0-A126-6EE1C0049348}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="1320" windowWidth="27675" windowHeight="13920" xr2:uid="{A3FA9652-9A23-4A5C-B165-97041DC41289}"/>
+    <workbookView xWindow="870" yWindow="780" windowWidth="26190" windowHeight="13920" xr2:uid="{A3FA9652-9A23-4A5C-B165-97041DC41289}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
   <si>
     <t>Oil &amp; Gas Equipment &amp;Services</t>
   </si>
@@ -274,16 +274,141 @@
   </si>
   <si>
     <t>Problems</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLC_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLF_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLI_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLK_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLP_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLRE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLU_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLV_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLY_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XME_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XNTK_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XBI_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XAR_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XOP_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XPH_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/DIA_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XWEB_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XTL_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XSW_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XTH_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XSD_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XRT_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XRE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/KIE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/KCE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/KBE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/SYE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/SPY_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/SLY_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/MDY_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XTN_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XHE_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XHS_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XLB_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XITK_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XHB_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>https://us.spdrs.com/site-content/xls/XES_All_Holdings.xls</t>
+  </si>
+  <si>
+    <t>Url</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -306,16 +431,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E13199-1FA2-4794-ADC7-CC76D869AD73}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,7 +768,7 @@
     <col min="2" max="2" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -650,11 +778,14 @@
       <c r="C1" t="s">
         <v>77</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -664,8 +795,11 @@
       <c r="C2">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -675,8 +809,11 @@
       <c r="C3">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -686,8 +823,11 @@
       <c r="C4">
         <v>96</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -697,8 +837,11 @@
       <c r="C5">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -708,8 +851,11 @@
       <c r="C6">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -719,8 +865,11 @@
       <c r="C7">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -730,8 +879,11 @@
       <c r="C8">
         <v>67</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
@@ -741,8 +893,11 @@
       <c r="C9">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -752,8 +907,11 @@
       <c r="C10">
         <v>42</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -763,8 +921,11 @@
       <c r="C11">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -774,8 +935,11 @@
       <c r="C12">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -785,8 +949,11 @@
       <c r="C13">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -796,8 +963,11 @@
       <c r="C14">
         <v>63</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
@@ -807,8 +977,11 @@
       <c r="C15">
         <v>64</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -818,8 +991,11 @@
       <c r="C16">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
@@ -829,8 +1005,11 @@
       <c r="C17">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>36</v>
       </c>
@@ -840,8 +1019,11 @@
       <c r="C18">
         <v>120</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
@@ -851,8 +1033,11 @@
       <c r="C19">
         <v>31</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F19" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -862,8 +1047,11 @@
       <c r="C20">
         <v>64</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
@@ -873,8 +1061,11 @@
       <c r="C21">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>44</v>
       </c>
@@ -884,8 +1075,11 @@
       <c r="C22">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
@@ -895,9 +1089,12 @@
       <c r="C23">
         <v>45</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1"/>
+      <c r="F23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>49</v>
       </c>
@@ -907,8 +1104,11 @@
       <c r="C24">
         <v>43</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -918,8 +1118,11 @@
       <c r="C25">
         <v>157</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
@@ -929,8 +1132,11 @@
       <c r="C26">
         <v>41</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>56</v>
       </c>
@@ -940,8 +1146,11 @@
       <c r="C27">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>58</v>
       </c>
@@ -951,8 +1160,11 @@
       <c r="C28">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>59</v>
       </c>
@@ -962,8 +1174,11 @@
       <c r="C29">
         <v>124</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>62</v>
       </c>
@@ -973,8 +1188,11 @@
       <c r="C30">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>64</v>
       </c>
@@ -984,8 +1202,11 @@
       <c r="C31">
         <v>55</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>65</v>
       </c>
@@ -995,8 +1216,11 @@
       <c r="C32">
         <v>88</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>71</v>
       </c>
@@ -1006,8 +1230,11 @@
       <c r="C33">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F33" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>72</v>
       </c>
@@ -1017,8 +1244,11 @@
       <c r="C34">
         <v>506</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F34" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>73</v>
       </c>
@@ -1028,8 +1258,11 @@
       <c r="C35">
         <v>602</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F35" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>74</v>
       </c>
@@ -1039,8 +1272,11 @@
       <c r="C36">
         <v>401</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>48</v>
       </c>
@@ -1050,11 +1286,14 @@
       <c r="C37">
         <v>42</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F37" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>5</v>
       </c>
@@ -1064,11 +1303,14 @@
       <c r="C38">
         <v>67</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -1078,11 +1320,54 @@
       <c r="C39">
         <v>37</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>79</v>
       </c>
+      <c r="F39" s="2" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{9D43F7CD-25AC-4A48-93C1-38B2E45490F9}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{41BB7FA1-0A79-43A3-A681-D4F04E18C508}"/>
+    <hyperlink ref="F8" r:id="rId3" xr:uid="{1F82B038-6554-4F4A-9C2D-10018DFF6854}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{E26633FE-E5F5-4BE6-8840-65F9A26D487C}"/>
+    <hyperlink ref="F10" r:id="rId5" xr:uid="{81B94D25-A29D-4804-8A60-6B3D93DD555D}"/>
+    <hyperlink ref="F11" r:id="rId6" xr:uid="{8D7E3D3F-CF47-49BB-B72A-FF231679F371}"/>
+    <hyperlink ref="F12" r:id="rId7" xr:uid="{3BB267DE-DFC4-4E1C-803D-4B3555FC9C5A}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{05F3027F-9DE4-4BF6-BDAA-74C0F54966ED}"/>
+    <hyperlink ref="F14" r:id="rId9" xr:uid="{E365FB2C-23E7-4B64-96E1-F8E66797883E}"/>
+    <hyperlink ref="F15" r:id="rId10" xr:uid="{662EE149-9AAF-48B1-8223-6AF8532F60F0}"/>
+    <hyperlink ref="F16" r:id="rId11" xr:uid="{AE75F8A6-708A-46ED-B93F-D691ADAA8606}"/>
+    <hyperlink ref="F17" r:id="rId12" xr:uid="{3A1A01C6-F721-469A-B388-08BDB1111219}"/>
+    <hyperlink ref="F18" r:id="rId13" xr:uid="{3626F337-97AE-426B-A4D6-52C72518E534}"/>
+    <hyperlink ref="F19" r:id="rId14" xr:uid="{7C1FE39F-15EF-4FEF-9785-665587EC7007}"/>
+    <hyperlink ref="F20" r:id="rId15" xr:uid="{A94B358D-890D-4FD3-90F5-1C8474DBB97D}"/>
+    <hyperlink ref="F21" r:id="rId16" xr:uid="{664248B6-7EB6-419F-8AA8-D9BD08ABDD1B}"/>
+    <hyperlink ref="F22" r:id="rId17" xr:uid="{AA4C72BE-9875-401A-AA92-26D227D2306F}"/>
+    <hyperlink ref="F23" r:id="rId18" xr:uid="{9974A899-3E5E-4B62-8228-1EFCA7669320}"/>
+    <hyperlink ref="F24" r:id="rId19" xr:uid="{A5D70A64-70C2-439E-8B97-46B3CB330959}"/>
+    <hyperlink ref="F25" r:id="rId20" xr:uid="{E81E8BDB-67B3-4870-8A39-211331C8ED68}"/>
+    <hyperlink ref="F26" r:id="rId21" xr:uid="{2833CE7F-8A98-4937-8A23-74CEBC25F56A}"/>
+    <hyperlink ref="F27" r:id="rId22" xr:uid="{C82AFAEA-2D0C-47E8-98F3-D83FFDA64DFB}"/>
+    <hyperlink ref="F28" r:id="rId23" xr:uid="{7F5C7E39-86CD-4162-9F7A-778E7E88D755}"/>
+    <hyperlink ref="F29" r:id="rId24" xr:uid="{7A0FD569-E817-4DAB-A420-D514E4632D82}"/>
+    <hyperlink ref="F30" r:id="rId25" xr:uid="{053D635C-9E67-46DC-87DA-3C2DF1E87258}"/>
+    <hyperlink ref="F31" r:id="rId26" xr:uid="{7FBCD6DF-C7F6-4E69-91A5-493F9313227D}"/>
+    <hyperlink ref="F32" r:id="rId27" xr:uid="{BD8E735C-1067-4968-AABA-AAB0BEA68266}"/>
+    <hyperlink ref="F33" r:id="rId28" xr:uid="{FFC1EA34-19E9-4CED-9BA1-CD9BDCE6899E}"/>
+    <hyperlink ref="F34" r:id="rId29" xr:uid="{D74F63E3-9B4C-4C09-A247-F10AF93FF59A}"/>
+    <hyperlink ref="F35" r:id="rId30" xr:uid="{BC871A9C-25B9-44C7-B470-E038D5B0A3F9}"/>
+    <hyperlink ref="F36" r:id="rId31" xr:uid="{11FB3532-6FEB-4147-9DB2-919D9431C33E}"/>
+    <hyperlink ref="F37" r:id="rId32" xr:uid="{22404435-6FB8-4921-AACD-089E29C90F2F}"/>
+    <hyperlink ref="F38" r:id="rId33" xr:uid="{0F7B146C-AE26-4AE0-B711-A8A000B1B864}"/>
+    <hyperlink ref="F39" r:id="rId34" xr:uid="{67A64367-81CB-4422-929D-CE75D9EB8DD3}"/>
+    <hyperlink ref="F5" r:id="rId35" xr:uid="{DE9672CB-8464-4DB6-973B-5D8262F01CCC}"/>
+    <hyperlink ref="F4" r:id="rId36" xr:uid="{940D8F2D-385F-4C28-B987-52F8446DFCDE}"/>
+    <hyperlink ref="F3" r:id="rId37" xr:uid="{ABEFC35F-4BFD-4153-9CB1-5F52C23074FD}"/>
+    <hyperlink ref="F2" r:id="rId38" xr:uid="{C59E4007-43DF-4D46-962B-503EEF57519C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>